<commit_message>
creation of a new route to search for products
</commit_message>
<xml_diff>
--- a/database/seeders/data/excel_green_plastic.xlsx
+++ b/database/seeders/data/excel_green_plastic.xlsx
@@ -889,6 +889,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -910,16 +911,19 @@
       <color rgb="FF000000"/>
       <name val="MS Sans Serif"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -932,7 +936,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.5999"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1018,52 +1022,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1092,7 +1100,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4C7E7"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1112,7 +1120,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF89FD78"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -1252,1647 +1260,1647 @@
   </sheetPr>
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D100" activeCellId="0" sqref="D100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C104" activeCellId="0" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="142.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="142.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="C23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="C35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="C38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" s="6" t="s">
+      <c r="C75" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="D76" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="E76" s="7" t="s">
+      <c r="E76" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="D77" s="6" t="s">
+      <c r="C77" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="E77" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D78" s="6" t="s">
+      <c r="C78" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E78" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D79" s="6" t="s">
+      <c r="C79" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="E79" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D80" s="4" t="s">
+      <c r="C80" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E80" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="D81" s="6" t="s">
+      <c r="C81" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D81" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="E81" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C82" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D82" s="6" t="s">
+      <c r="C82" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D82" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="E82" s="7" t="s">
+      <c r="E82" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D83" s="4" t="s">
+      <c r="C83" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E83" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B84" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C84" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="D84" s="6" t="s">
+      <c r="C84" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E84" s="7" t="s">
+      <c r="E84" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="C85" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D85" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D86" s="4" t="s">
+      <c r="C86" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E86" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D87" s="4" t="s">
+      <c r="C87" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="D88" s="4" t="s">
+      <c r="C88" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D89" s="4" t="s">
+      <c r="C89" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="D90" s="4" t="s">
+      <c r="C90" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E90" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D91" s="4" t="s">
+      <c r="C91" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E91" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="D92" s="4" t="s">
+      <c r="C92" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E92" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D93" s="4" t="s">
+      <c r="C93" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E93" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C94" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="D94" s="4" t="s">
+      <c r="C94" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="C95" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D95" s="4" t="s">
+      <c r="C95" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E95" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="C96" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="D96" s="4" t="s">
+      <c r="C96" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="E96" s="12" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>